<commit_message>
updates to census_sources.xlsx files
</commit_message>
<xml_diff>
--- a/Sean/census_sources.xlsx
+++ b/Sean/census_sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevineliasen/GoogleDrive/CodingStuff/Gits/via_datas/VIA_project/kevin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17561DC-DAA5-B144-8528-C25EB7FD74DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E6372E-BD20-A447-9FED-53AA561C0721}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,16 +18,20 @@
     <sheet name="field_log" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="api_url">url_builder!$B$1</definedName>
-    <definedName name="field_id">url_builder!$F$8:$F$37</definedName>
-    <definedName name="field_number">url_builder!$E$8:$E$37</definedName>
-    <definedName name="group_letter">url_builder!$A$8:$A$37</definedName>
-    <definedName name="group_number">url_builder!$B$8:$B$37</definedName>
-    <definedName name="group_sub">url_builder!$C$8:$C$37</definedName>
-    <definedName name="link_prep">url_builder!$G$8:$G$37</definedName>
-    <definedName name="search_type">url_builder!$D$8:$D$37</definedName>
-    <definedName name="url_middle">url_builder!$B$4</definedName>
-    <definedName name="url_prefix">url_builder!$B$3</definedName>
+    <definedName name="api_url">url_builder!$B$2</definedName>
+    <definedName name="field_id">url_builder!$F$13:$F$62</definedName>
+    <definedName name="field_number">url_builder!$D$13:$D$62</definedName>
+    <definedName name="group_letter">url_builder!$A$13:$A$62</definedName>
+    <definedName name="group_number">url_builder!$B$13:$B$62</definedName>
+    <definedName name="group_sub">url_builder!$C$13:$C$62</definedName>
+    <definedName name="https___api.census.gov_data_2018">url_builder!$P$5:$P$9</definedName>
+    <definedName name="link_prep">url_builder!$G$13:$G$62</definedName>
+    <definedName name="search_type">url_builder!$E$13:$E$62</definedName>
+    <definedName name="url_base">url_builder!$P$4</definedName>
+    <definedName name="url_for">url_builder!$P$8</definedName>
+    <definedName name="url_get">url_builder!$P$6</definedName>
+    <definedName name="url_in">url_builder!$P$9</definedName>
+    <definedName name="url_report">url_builder!$P$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,8 +47,321 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Kevin Eliasen</author>
+  </authors>
+  <commentList>
+    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{4FFA9E4F-A250-944A-B06D-52AA90A05AA2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kevin Eliasen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Alpha, 1 character, required</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{54BD7CC2-5BBE-3E47-A488-8684412C461D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kevin Eliasen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Numeric, up to 5 characters, required</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{3BDBBD33-22CF-6549-A334-78604CEABE3C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kevin Eliasen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Alpha, 1 character
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>OPTIONAL - used in select groups where Census data is subdivided, usually by race</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{E88443AB-C09A-B749-BF5B-5BD2540E0675}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kevin Eliasen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">numeric, 1-999
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">All rows with a value in this field will be included in API get call.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Blank rows will be EXCLUDED</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{7FB3A44E-5757-E14E-B335-273D08ADE25A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kevin Eliasen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Alpha, 1 character, required, default="E"
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Generally no need to change this value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{6B0B2F87-1A9D-DE47-8AE3-D4F67185BCF5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kevin Eliasen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Field ID as defined by Census API.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Must match exactly</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G12" authorId="0" shapeId="0" xr:uid="{0D7165D6-7C9E-4342-B099-F2C1A1B25059}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kevin Eliasen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">This column is for URL building only.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DO NOT MEDDLE WITH THIS COLUMN</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="260">
   <si>
     <t>B01001_001E</t>
   </si>
@@ -700,21 +1017,9 @@
     <t>C17002_008E</t>
   </si>
   <si>
-    <t>url_prefix</t>
-  </si>
-  <si>
-    <t>https://api.census.gov/data/2018/acs/acs5?get=</t>
-  </si>
-  <si>
-    <t>url_middle</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
-    <t>I</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
@@ -746,13 +1051,213 @@
   </si>
   <si>
     <t>group_desc</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>url_for</t>
+  </si>
+  <si>
+    <t>url_in</t>
+  </si>
+  <si>
+    <t>url_report</t>
+  </si>
+  <si>
+    <t>url_get</t>
+  </si>
+  <si>
+    <t>/acs/acs5</t>
+  </si>
+  <si>
+    <t>https://api.census.gov/data/2018</t>
+  </si>
+  <si>
+    <t>&amp;in=state:48&amp;in=county:029&amp;in=tract:*</t>
+  </si>
+  <si>
+    <t>&amp;for=block%20group:*</t>
+  </si>
+  <si>
+    <t>url_base</t>
+  </si>
+  <si>
+    <t>EXAMPLE</t>
+  </si>
+  <si>
+    <t>B11001_001E</t>
+  </si>
+  <si>
+    <t>B11001A_001E</t>
+  </si>
+  <si>
+    <t>&lt; blank &gt;</t>
+  </si>
+  <si>
+    <t>Census API URL builder</t>
+  </si>
+  <si>
+    <t>INSTRUCTIONS</t>
+  </si>
+  <si>
+    <t>Not OK to Edit</t>
+  </si>
+  <si>
+    <t>OK to Edit</t>
+  </si>
+  <si>
+    <t>Use top row to input group information and the first field number to be queried. Fill additional field numbers as needed in subsequent rows.</t>
+  </si>
+  <si>
+    <t>Changes can be made to maroon fields, however these should be overwritten with the original formulae once hyperlink is bult</t>
+  </si>
+  <si>
+    <t>All calculated component fields pull the value from the record directly above them. If hard-coded values are necessary, limit changes to first where change should occur</t>
+  </si>
+  <si>
+    <t>OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</t>
+  </si>
+  <si>
+    <t>FORMULA</t>
+  </si>
+  <si>
+    <t>Conditional formatting will show columns where formulae need to be replaced</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Active hyperlink will be created in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>api_url</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> field (B2).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Census API will error if any unknown fields are presented. Check the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>field_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> column.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Copy used </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>field_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> values to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>field_log</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> worksheet or other documentation file.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Copy value of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>api_url</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> field to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>grouping_url_log</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> sheet or other documentation file.</t>
+    </r>
+  </si>
+  <si>
+    <t>API Components</t>
+  </si>
+  <si>
+    <t>no touchy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -787,14 +1292,15 @@
       <name val="Inconsolata"/>
     </font>
     <font>
+      <u/>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Roboto"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
-      <color rgb="FF0000FF"/>
+      <color theme="10"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -830,6 +1336,66 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FFFFC000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -857,7 +1423,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -865,11 +1431,104 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -877,8 +1536,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -902,11 +1560,188 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color theme="5" tint="0.39994506668294322"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="0.39994506668294322"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="0.39994506668294322"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="0.39994506668294322"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="0.39994506668294322"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="0.39994506668294322"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="0.39994506668294322"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -917,6 +1752,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1116,896 +1955,1724 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:S62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="8" max="8" width="3.5" customWidth="1"/>
+    <col min="14" max="14" width="3.33203125" customWidth="1"/>
+    <col min="16" max="16" width="43.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:19" ht="28">
+      <c r="A1" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="I1" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="O1" s="28" t="s">
+        <v>258</v>
+      </c>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+    </row>
+    <row r="2" spans="1:19" ht="15" customHeight="1">
+      <c r="A2" s="29" t="s">
+        <v>227</v>
+      </c>
+      <c r="B2" s="30" t="str">
+        <f ca="1">HYPERLINK(url_base&amp;url_report&amp;url_get&amp;url_for&amp;url_in)</f>
+        <v>https://api.census.gov/data/2018/acs/acs5?get=B11001_001E,B11001_002E,B11001_003E,B11001_004E,B11001_005E,B11001_006E,B11001_007E,B11001_008E,B11001_009E&amp;for=block%20group:*&amp;in=state:48&amp;in=county:029&amp;in=tract:*</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="I2" s="31" t="s">
+        <v>248</v>
+      </c>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="O2" s="44" t="s">
+        <v>259</v>
+      </c>
+      <c r="P2" s="44"/>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
+      <c r="A3" s="29"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+    </row>
+    <row r="4" spans="1:19" ht="15" customHeight="1">
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="I4" s="31" t="s">
+        <v>254</v>
+      </c>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="O4" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="P4" s="19" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15" customHeight="1">
+      <c r="F5" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="I5" s="31" t="s">
+        <v>255</v>
+      </c>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="O5" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="P5" s="18" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15" customHeight="1" thickBot="1">
+      <c r="A6" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="I6" s="31" t="s">
+        <v>257</v>
+      </c>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="O6" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="P6" s="43" t="str">
+        <f ca="1">IF(G13&amp;""="","","?get="&amp;G13)</f>
+        <v>?get=B11001_001E,B11001_002E,B11001_003E,B11001_004E,B11001_005E,B11001_006E,B11001_007E,B11001_008E,B11001_009E</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15" customHeight="1">
+      <c r="A7" s="33" t="s">
+        <v>220</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>221</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>222</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="E7" s="34" t="s">
+        <v>223</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>225</v>
+      </c>
+      <c r="I7" s="31" t="s">
+        <v>256</v>
+      </c>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="P7" s="43"/>
+    </row>
+    <row r="8" spans="1:19" ht="15.75" customHeight="1">
+      <c r="A8" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="B8" s="25">
+        <v>11001</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>243</v>
+      </c>
+      <c r="D8" s="25">
+        <v>1</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="I8" s="31" t="s">
+        <v>249</v>
+      </c>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="O8" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="B1" s="8" t="str">
-        <f>B3&amp;G8&amp;B4</f>
-        <v>https://api.census.gov/data/2018/acs/acs5?get=B11001I_001E,B11001I_002E,B11001I_003E,B11001I_004E,B11001I_005E,B11001I_006E,B11001I_007E,B11001I_008E,B11001I_009E&amp;for=block%20group:*&amp;in=state:48&amp;in=county:029&amp;in=tract:*</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A3" s="11" t="s">
+      <c r="P8" s="20" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="15.75" customHeight="1">
+      <c r="A9" s="36" t="s">
         <v>218</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B9" s="25">
+        <v>11001</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="D9" s="25">
+        <v>1</v>
+      </c>
+      <c r="E9" s="23" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A4" s="11" t="s">
+      <c r="F9" s="37" t="s">
+        <v>242</v>
+      </c>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="O9" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A10" s="38" t="s">
+        <v>218</v>
+      </c>
+      <c r="B10" s="39">
+        <v>11001</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>243</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>243</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>219</v>
+      </c>
+      <c r="F10" s="42" t="s">
+        <v>243</v>
+      </c>
+      <c r="I10" s="31" t="s">
+        <v>250</v>
+      </c>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+    </row>
+    <row r="11" spans="1:19" ht="15.75" customHeight="1">
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+    </row>
+    <row r="12" spans="1:19" ht="15.75" customHeight="1">
+      <c r="A12" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="B4" s="5" t="str">
-        <f>"&amp;for=block%20group:*&amp;in=state:48&amp;in=county:029&amp;in=tract:*"</f>
-        <v>&amp;for=block%20group:*&amp;in=state:48&amp;in=county:029&amp;in=tract:*</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B5" s="1"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A7" s="9" t="s">
+      <c r="B12" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="E12" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="G12" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>229</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A8" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="B8" s="12">
-        <v>11001</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>222</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>223</v>
-      </c>
-      <c r="E8" s="13">
+      <c r="I12" s="32" t="s">
+        <v>253</v>
+      </c>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
+    </row>
+    <row r="13" spans="1:19" ht="15.75" customHeight="1">
+      <c r="A13" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="B13" s="11">
+        <v>11001</v>
+      </c>
+      <c r="C13" s="17"/>
+      <c r="D13" s="12">
         <v>1</v>
       </c>
-      <c r="F8" s="10" t="str">
-        <f>IF($E8="","",A8&amp;RIGHT("00000"&amp;B8,5)&amp;C8&amp;"_"&amp;RIGHT("000"&amp;E8,3)&amp;D8)</f>
-        <v>B11001I_001E</v>
-      </c>
-      <c r="G8" s="14" t="str">
-        <f>IF($E8="",G9,F8&amp;IF(G9="","",IF(OR(G9=0,G9=""),"",","&amp;G9)))</f>
-        <v>B11001I_001E,B11001I_002E,B11001I_003E,B11001I_004E,B11001I_005E,B11001I_006E,B11001I_007E,B11001I_008E,B11001I_009E</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A9" s="15" t="str">
-        <f>IF($E9="","",A$8)</f>
+      <c r="E13" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="F13" s="9" t="str">
+        <f>IF($D13="","",A13&amp;RIGHT("00000"&amp;B13,5)&amp;C13&amp;"_"&amp;RIGHT("000"&amp;D13,3)&amp;E13)</f>
+        <v>B11001_001E</v>
+      </c>
+      <c r="G13" s="13" t="str">
+        <f ca="1">IF($D13="",G14&amp;"",F13&amp;IF(G14="","",IF(OR(G14=0,G14=""),"",","&amp;G14)))</f>
+        <v>B11001_001E,B11001_002E,B11001_003E,B11001_004E,B11001_005E,B11001_006E,B11001_007E,B11001_008E,B11001_009E</v>
+      </c>
+      <c r="I13" s="21" t="s">
+        <v>252</v>
+      </c>
+      <c r="J13" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="15.75" customHeight="1">
+      <c r="A14" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A14" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
         <v>B</v>
       </c>
-      <c r="B9" s="15">
-        <f>IF($E9="","",B$8)</f>
-        <v>11001</v>
-      </c>
-      <c r="C9" s="15" t="str">
-        <f>IF($E9="","",C8)</f>
-        <v>I</v>
-      </c>
-      <c r="D9" s="15" t="str">
-        <f>IF($E9="","",D$8)</f>
+      <c r="B14" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B14" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C14" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C14" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D14" s="12">
+        <v>2</v>
+      </c>
+      <c r="E14" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E14" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
         <v>E</v>
       </c>
-      <c r="E9" s="13">
-        <v>2</v>
-      </c>
-      <c r="F9" s="10" t="str">
-        <f t="shared" ref="F9:F37" si="0">IF($E9="","",A9&amp;RIGHT("00000"&amp;B9,5)&amp;C9&amp;"_"&amp;RIGHT("000"&amp;E9,3)&amp;D9)</f>
-        <v>B11001I_002E</v>
-      </c>
-      <c r="G9" s="14" t="str">
-        <f t="shared" ref="G9:G37" si="1">IF($E9="",G10,F9&amp;IF(G10="","",IF(OR(G10=0,G10=""),"",","&amp;G10)))</f>
-        <v>B11001I_002E,B11001I_003E,B11001I_004E,B11001I_005E,B11001I_006E,B11001I_007E,B11001I_008E,B11001I_009E</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A10" s="15" t="str">
-        <f>IF($E10="","",A9)</f>
+      <c r="F14" s="9" t="str">
+        <f ca="1">IF($D14="","",A14&amp;RIGHT("00000"&amp;B14,5)&amp;C14&amp;"_"&amp;RIGHT("000"&amp;D14,3)&amp;E14)</f>
+        <v>B11001_002E</v>
+      </c>
+      <c r="G14" s="13" t="str">
+        <f ca="1">IF($D14="",G15&amp;"",F14&amp;IF(G15="","",IF(OR(G15=0,G15=""),"",","&amp;G15)))</f>
+        <v>B11001_002E,B11001_003E,B11001_004E,B11001_005E,B11001_006E,B11001_007E,B11001_008E,B11001_009E</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="15.75" customHeight="1">
+      <c r="A15" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A15" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
         <v>B</v>
       </c>
-      <c r="B10" s="15">
-        <f>IF($E10="","",B9)</f>
-        <v>11001</v>
-      </c>
-      <c r="C10" s="15" t="str">
-        <f>IF($E10="","",C9)</f>
-        <v>I</v>
-      </c>
-      <c r="D10" s="15" t="str">
-        <f>IF($E10="","",D9)</f>
+      <c r="B15" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B15" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C15" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C15" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D15" s="12">
+        <v>3</v>
+      </c>
+      <c r="E15" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E15" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
         <v>E</v>
       </c>
-      <c r="E10" s="13">
-        <v>3</v>
-      </c>
-      <c r="F10" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>B11001I_003E</v>
-      </c>
-      <c r="G10" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>B11001I_003E,B11001I_004E,B11001I_005E,B11001I_006E,B11001I_007E,B11001I_008E,B11001I_009E</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A11" s="15" t="str">
-        <f>IF($E11="","",A10)</f>
+      <c r="F15" s="9" t="str">
+        <f ca="1">IF($D15="","",A15&amp;RIGHT("00000"&amp;B15,5)&amp;C15&amp;"_"&amp;RIGHT("000"&amp;D15,3)&amp;E15)</f>
+        <v>B11001_003E</v>
+      </c>
+      <c r="G15" s="13" t="str">
+        <f ca="1">IF($D15="",G16&amp;"",F15&amp;IF(G16="","",IF(OR(G16=0,G16=""),"",","&amp;G16)))</f>
+        <v>B11001_003E,B11001_004E,B11001_005E,B11001_006E,B11001_007E,B11001_008E,B11001_009E</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="15.75" customHeight="1">
+      <c r="A16" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A16" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
         <v>B</v>
       </c>
-      <c r="B11" s="15">
-        <f>IF($E11="","",B10)</f>
-        <v>11001</v>
-      </c>
-      <c r="C11" s="15" t="str">
-        <f>IF($E11="","",C10)</f>
-        <v>I</v>
-      </c>
-      <c r="D11" s="15" t="str">
-        <f>IF($E11="","",D10)</f>
+      <c r="B16" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B16" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C16" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C16" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D16" s="12">
+        <v>4</v>
+      </c>
+      <c r="E16" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E16" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
         <v>E</v>
       </c>
-      <c r="E11" s="13">
-        <v>4</v>
-      </c>
-      <c r="F11" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>B11001I_004E</v>
-      </c>
-      <c r="G11" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>B11001I_004E,B11001I_005E,B11001I_006E,B11001I_007E,B11001I_008E,B11001I_009E</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A12" s="15" t="str">
-        <f>IF($E12="","",A11)</f>
+      <c r="F16" s="9" t="str">
+        <f ca="1">IF($D16="","",A16&amp;RIGHT("00000"&amp;B16,5)&amp;C16&amp;"_"&amp;RIGHT("000"&amp;D16,3)&amp;E16)</f>
+        <v>B11001_004E</v>
+      </c>
+      <c r="G16" s="13" t="str">
+        <f ca="1">IF($D16="",G17&amp;"",F16&amp;IF(G17="","",IF(OR(G17=0,G17=""),"",","&amp;G17)))</f>
+        <v>B11001_004E,B11001_005E,B11001_006E,B11001_007E,B11001_008E,B11001_009E</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A17" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A17" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
         <v>B</v>
       </c>
-      <c r="B12" s="15">
-        <f>IF($E12="","",B11)</f>
-        <v>11001</v>
-      </c>
-      <c r="C12" s="15" t="str">
-        <f>IF($E12="","",C11)</f>
-        <v>I</v>
-      </c>
-      <c r="D12" s="15" t="str">
-        <f>IF($E12="","",D11)</f>
+      <c r="B17" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B17" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C17" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C17" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D17" s="12">
+        <v>5</v>
+      </c>
+      <c r="E17" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E17" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
         <v>E</v>
       </c>
-      <c r="E12" s="13">
-        <v>5</v>
-      </c>
-      <c r="F12" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>B11001I_005E</v>
-      </c>
-      <c r="G12" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>B11001I_005E,B11001I_006E,B11001I_007E,B11001I_008E,B11001I_009E</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A13" s="15" t="str">
-        <f>IF($E13="","",A12)</f>
+      <c r="F17" s="9" t="str">
+        <f ca="1">IF($D17="","",A17&amp;RIGHT("00000"&amp;B17,5)&amp;C17&amp;"_"&amp;RIGHT("000"&amp;D17,3)&amp;E17)</f>
+        <v>B11001_005E</v>
+      </c>
+      <c r="G17" s="13" t="str">
+        <f ca="1">IF($D17="",G18&amp;"",F17&amp;IF(G18="","",IF(OR(G18=0,G18=""),"",","&amp;G18)))</f>
+        <v>B11001_005E,B11001_006E,B11001_007E,B11001_008E,B11001_009E</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A18" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A18" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
         <v>B</v>
       </c>
-      <c r="B13" s="15">
-        <f>IF($E13="","",B12)</f>
-        <v>11001</v>
-      </c>
-      <c r="C13" s="15" t="str">
-        <f>IF($E13="","",C12)</f>
-        <v>I</v>
-      </c>
-      <c r="D13" s="15" t="str">
-        <f>IF($E13="","",D12)</f>
+      <c r="B18" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B18" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C18" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C18" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D18" s="12">
+        <v>6</v>
+      </c>
+      <c r="E18" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E18" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
         <v>E</v>
       </c>
-      <c r="E13" s="13">
-        <v>6</v>
-      </c>
-      <c r="F13" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>B11001I_006E</v>
-      </c>
-      <c r="G13" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>B11001I_006E,B11001I_007E,B11001I_008E,B11001I_009E</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A14" s="15" t="str">
-        <f>IF($E14="","",A13)</f>
+      <c r="F18" s="9" t="str">
+        <f ca="1">IF($D18="","",A18&amp;RIGHT("00000"&amp;B18,5)&amp;C18&amp;"_"&amp;RIGHT("000"&amp;D18,3)&amp;E18)</f>
+        <v>B11001_006E</v>
+      </c>
+      <c r="G18" s="13" t="str">
+        <f ca="1">IF($D18="",G19&amp;"",F18&amp;IF(G19="","",IF(OR(G19=0,G19=""),"",","&amp;G19)))</f>
+        <v>B11001_006E,B11001_007E,B11001_008E,B11001_009E</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A19" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A19" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
         <v>B</v>
       </c>
-      <c r="B14" s="15">
-        <f>IF($E14="","",B13)</f>
-        <v>11001</v>
-      </c>
-      <c r="C14" s="15" t="str">
-        <f>IF($E14="","",C13)</f>
-        <v>I</v>
-      </c>
-      <c r="D14" s="15" t="str">
-        <f>IF($E14="","",D13)</f>
+      <c r="B19" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B19" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C19" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C19" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D19" s="12">
+        <v>7</v>
+      </c>
+      <c r="E19" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E19" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
         <v>E</v>
       </c>
-      <c r="E14" s="13">
-        <v>7</v>
-      </c>
-      <c r="F14" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>B11001I_007E</v>
-      </c>
-      <c r="G14" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>B11001I_007E,B11001I_008E,B11001I_009E</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A15" s="15" t="str">
-        <f>IF($E15="","",A14)</f>
+      <c r="F19" s="9" t="str">
+        <f ca="1">IF($D19="","",A19&amp;RIGHT("00000"&amp;B19,5)&amp;C19&amp;"_"&amp;RIGHT("000"&amp;D19,3)&amp;E19)</f>
+        <v>B11001_007E</v>
+      </c>
+      <c r="G19" s="13" t="str">
+        <f ca="1">IF($D19="",G20&amp;"",F19&amp;IF(G20="","",IF(OR(G20=0,G20=""),"",","&amp;G20)))</f>
+        <v>B11001_007E,B11001_008E,B11001_009E</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A20" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A20" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
         <v>B</v>
       </c>
-      <c r="B15" s="15">
-        <f>IF($E15="","",B14)</f>
-        <v>11001</v>
-      </c>
-      <c r="C15" s="15" t="str">
-        <f>IF($E15="","",C14)</f>
-        <v>I</v>
-      </c>
-      <c r="D15" s="15" t="str">
-        <f>IF($E15="","",D14)</f>
+      <c r="B20" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B20" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C20" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C20" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D20" s="12">
+        <v>8</v>
+      </c>
+      <c r="E20" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E20" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
         <v>E</v>
       </c>
-      <c r="E15" s="13">
-        <v>8</v>
-      </c>
-      <c r="F15" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>B11001I_008E</v>
-      </c>
-      <c r="G15" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>B11001I_008E,B11001I_009E</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A16" s="15" t="str">
-        <f>IF($E16="","",A15)</f>
+      <c r="F20" s="9" t="str">
+        <f ca="1">IF($D20="","",A20&amp;RIGHT("00000"&amp;B20,5)&amp;C20&amp;"_"&amp;RIGHT("000"&amp;D20,3)&amp;E20)</f>
+        <v>B11001_008E</v>
+      </c>
+      <c r="G20" s="13" t="str">
+        <f ca="1">IF($D20="",G21&amp;"",F20&amp;IF(G21="","",IF(OR(G21=0,G21=""),"",","&amp;G21)))</f>
+        <v>B11001_008E,B11001_009E</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A21" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A21" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
         <v>B</v>
       </c>
-      <c r="B16" s="15">
-        <f>IF($E16="","",B15)</f>
-        <v>11001</v>
-      </c>
-      <c r="C16" s="15" t="str">
-        <f>IF($E16="","",C15)</f>
-        <v>I</v>
-      </c>
-      <c r="D16" s="15" t="str">
-        <f>IF($E16="","",D15)</f>
+      <c r="B21" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B21" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C21" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C21" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D21" s="12">
+        <v>9</v>
+      </c>
+      <c r="E21" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E21" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
         <v>E</v>
       </c>
-      <c r="E16" s="13">
-        <v>9</v>
-      </c>
-      <c r="F16" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>B11001I_009E</v>
-      </c>
-      <c r="G16" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>B11001I_009E</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A17" s="15" t="str">
-        <f>IF($E17="","",A16)</f>
-        <v/>
-      </c>
-      <c r="B17" s="15" t="str">
-        <f>IF($E17="","",B16)</f>
-        <v/>
-      </c>
-      <c r="C17" s="15" t="str">
-        <f>IF($E17="","",C16)</f>
-        <v/>
-      </c>
-      <c r="D17" s="15" t="str">
-        <f>IF($E17="","",D16)</f>
-        <v/>
-      </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G17" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A18" s="15" t="str">
-        <f>IF($E18="","",A17)</f>
-        <v/>
-      </c>
-      <c r="B18" s="15" t="str">
-        <f>IF($E18="","",B17)</f>
-        <v/>
-      </c>
-      <c r="C18" s="15" t="str">
-        <f>IF($E18="","",C17)</f>
-        <v/>
-      </c>
-      <c r="D18" s="15" t="str">
-        <f>IF($E18="","",D17)</f>
-        <v/>
-      </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G18" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A19" s="15" t="str">
-        <f>IF($E19="","",A18)</f>
-        <v/>
-      </c>
-      <c r="B19" s="15" t="str">
-        <f>IF($E19="","",B18)</f>
-        <v/>
-      </c>
-      <c r="C19" s="15" t="str">
-        <f>IF($E19="","",C18)</f>
-        <v/>
-      </c>
-      <c r="D19" s="15" t="str">
-        <f>IF($E19="","",D18)</f>
-        <v/>
-      </c>
-      <c r="E19" s="16"/>
-      <c r="F19" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G19" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A20" s="15" t="str">
-        <f>IF($E20="","",A19)</f>
-        <v/>
-      </c>
-      <c r="B20" s="15" t="str">
-        <f>IF($E20="","",B19)</f>
-        <v/>
-      </c>
-      <c r="C20" s="15" t="str">
-        <f>IF($E20="","",C19)</f>
-        <v/>
-      </c>
-      <c r="D20" s="15" t="str">
-        <f>IF($E20="","",D19)</f>
-        <v/>
-      </c>
-      <c r="E20" s="16"/>
-      <c r="F20" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G20" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A21" s="15" t="str">
-        <f>IF($E21="","",A20)</f>
-        <v/>
-      </c>
-      <c r="B21" s="15" t="str">
-        <f>IF($E21="","",B20)</f>
-        <v/>
-      </c>
-      <c r="C21" s="15" t="str">
-        <f>IF($E21="","",C20)</f>
-        <v/>
-      </c>
-      <c r="D21" s="15" t="str">
-        <f>IF($E21="","",D20)</f>
-        <v/>
-      </c>
-      <c r="E21" s="16"/>
-      <c r="F21" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G21" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F21" s="9" t="str">
+        <f ca="1">IF($D21="","",A21&amp;RIGHT("00000"&amp;B21,5)&amp;C21&amp;"_"&amp;RIGHT("000"&amp;D21,3)&amp;E21)</f>
+        <v>B11001_009E</v>
+      </c>
+      <c r="G21" s="13" t="str">
+        <f ca="1">IF($D21="",G22&amp;"",F21&amp;IF(G22="","",IF(OR(G22=0,G22=""),"",","&amp;G22)))</f>
+        <v>B11001_009E</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A22" s="15" t="str">
-        <f>IF($E22="","",A21)</f>
-        <v/>
-      </c>
-      <c r="B22" s="15" t="str">
-        <f>IF($E22="","",B21)</f>
-        <v/>
-      </c>
-      <c r="C22" s="15" t="str">
-        <f>IF($E22="","",C21)</f>
-        <v/>
-      </c>
-      <c r="D22" s="15" t="str">
-        <f>IF($E22="","",D21)</f>
-        <v/>
-      </c>
-      <c r="E22" s="16"/>
-      <c r="F22" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G22" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="A22" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A22" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B22" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B22" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C22" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C22" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D22" s="12"/>
+      <c r="E22" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E22" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F22" s="9" t="str">
+        <f>IF($D22="","",A22&amp;RIGHT("00000"&amp;B22,5)&amp;C22&amp;"_"&amp;RIGHT("000"&amp;D22,3)&amp;E22)</f>
+        <v/>
+      </c>
+      <c r="G22" s="13" t="str">
+        <f>IF($D22="",G23&amp;"",F22&amp;IF(G23="","",IF(OR(G23=0,G23=""),"",","&amp;G23)))</f>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A23" s="15" t="str">
-        <f>IF($E23="","",A22)</f>
-        <v/>
-      </c>
-      <c r="B23" s="15" t="str">
-        <f>IF($E23="","",B22)</f>
-        <v/>
-      </c>
-      <c r="C23" s="15" t="str">
-        <f>IF($E23="","",C22)</f>
-        <v/>
-      </c>
-      <c r="D23" s="15" t="str">
-        <f>IF($E23="","",D22)</f>
-        <v/>
-      </c>
-      <c r="E23" s="16"/>
-      <c r="F23" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G23" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="A23" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A23" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B23" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B23" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C23" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C23" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D23" s="12"/>
+      <c r="E23" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E23" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F23" s="9" t="str">
+        <f>IF($D23="","",A23&amp;RIGHT("00000"&amp;B23,5)&amp;C23&amp;"_"&amp;RIGHT("000"&amp;D23,3)&amp;E23)</f>
+        <v/>
+      </c>
+      <c r="G23" s="13" t="str">
+        <f>IF($D23="",G24&amp;"",F23&amp;IF(G24="","",IF(OR(G24=0,G24=""),"",","&amp;G24)))</f>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A24" s="15" t="str">
-        <f>IF($E24="","",A23)</f>
-        <v/>
-      </c>
-      <c r="B24" s="15" t="str">
-        <f>IF($E24="","",B23)</f>
-        <v/>
-      </c>
-      <c r="C24" s="15" t="str">
-        <f>IF($E24="","",C23)</f>
-        <v/>
-      </c>
-      <c r="D24" s="15" t="str">
-        <f>IF($E24="","",D23)</f>
-        <v/>
-      </c>
-      <c r="E24" s="16"/>
-      <c r="F24" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G24" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="A24" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A24" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B24" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B24" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C24" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C24" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D24" s="12"/>
+      <c r="E24" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E24" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F24" s="9" t="str">
+        <f>IF($D24="","",A24&amp;RIGHT("00000"&amp;B24,5)&amp;C24&amp;"_"&amp;RIGHT("000"&amp;D24,3)&amp;E24)</f>
+        <v/>
+      </c>
+      <c r="G24" s="13" t="str">
+        <f>IF($D24="",G25&amp;"",F24&amp;IF(G25="","",IF(OR(G25=0,G25=""),"",","&amp;G25)))</f>
+        <v/>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A25" s="15" t="str">
-        <f>IF($E25="","",A24)</f>
-        <v/>
-      </c>
-      <c r="B25" s="15" t="str">
-        <f>IF($E25="","",B24)</f>
-        <v/>
-      </c>
-      <c r="C25" s="15" t="str">
-        <f>IF($E25="","",C24)</f>
-        <v/>
-      </c>
-      <c r="D25" s="15" t="str">
-        <f>IF($E25="","",D24)</f>
-        <v/>
-      </c>
-      <c r="E25" s="16"/>
-      <c r="F25" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G25" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="A25" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A25" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B25" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B25" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C25" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C25" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D25" s="12"/>
+      <c r="E25" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E25" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F25" s="9" t="str">
+        <f>IF($D25="","",A25&amp;RIGHT("00000"&amp;B25,5)&amp;C25&amp;"_"&amp;RIGHT("000"&amp;D25,3)&amp;E25)</f>
+        <v/>
+      </c>
+      <c r="G25" s="13" t="str">
+        <f>IF($D25="",G26&amp;"",F25&amp;IF(G26="","",IF(OR(G26=0,G26=""),"",","&amp;G26)))</f>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A26" s="15" t="str">
-        <f>IF($E26="","",A25)</f>
-        <v/>
-      </c>
-      <c r="B26" s="15" t="str">
-        <f>IF($E26="","",B25)</f>
-        <v/>
-      </c>
-      <c r="C26" s="15" t="str">
-        <f>IF($E26="","",C25)</f>
-        <v/>
-      </c>
-      <c r="D26" s="15" t="str">
-        <f>IF($E26="","",D25)</f>
-        <v/>
-      </c>
-      <c r="E26" s="16"/>
-      <c r="F26" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G26" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="A26" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A26" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B26" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B26" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C26" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C26" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D26" s="12"/>
+      <c r="E26" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E26" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F26" s="9" t="str">
+        <f>IF($D26="","",A26&amp;RIGHT("00000"&amp;B26,5)&amp;C26&amp;"_"&amp;RIGHT("000"&amp;D26,3)&amp;E26)</f>
+        <v/>
+      </c>
+      <c r="G26" s="13" t="str">
+        <f>IF($D26="",G27&amp;"",F26&amp;IF(G27="","",IF(OR(G27=0,G27=""),"",","&amp;G27)))</f>
+        <v/>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A27" s="15" t="str">
-        <f>IF($E27="","",A26)</f>
-        <v/>
-      </c>
-      <c r="B27" s="15" t="str">
-        <f>IF($E27="","",B26)</f>
-        <v/>
-      </c>
-      <c r="C27" s="15" t="str">
-        <f>IF($E27="","",C26)</f>
-        <v/>
-      </c>
-      <c r="D27" s="15" t="str">
-        <f>IF($E27="","",D26)</f>
-        <v/>
-      </c>
-      <c r="E27" s="16"/>
-      <c r="F27" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G27" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="A27" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A27" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B27" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B27" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C27" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C27" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D27" s="12"/>
+      <c r="E27" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E27" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F27" s="9" t="str">
+        <f>IF($D27="","",A27&amp;RIGHT("00000"&amp;B27,5)&amp;C27&amp;"_"&amp;RIGHT("000"&amp;D27,3)&amp;E27)</f>
+        <v/>
+      </c>
+      <c r="G27" s="13" t="str">
+        <f>IF($D27="",G28&amp;"",F27&amp;IF(G28="","",IF(OR(G28=0,G28=""),"",","&amp;G28)))</f>
+        <v/>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A28" s="15" t="str">
-        <f>IF($E28="","",A27)</f>
-        <v/>
-      </c>
-      <c r="B28" s="15" t="str">
-        <f>IF($E28="","",B27)</f>
-        <v/>
-      </c>
-      <c r="C28" s="15" t="str">
-        <f>IF($E28="","",C27)</f>
-        <v/>
-      </c>
-      <c r="D28" s="15" t="str">
-        <f>IF($E28="","",D27)</f>
-        <v/>
-      </c>
-      <c r="E28" s="16"/>
-      <c r="F28" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G28" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="A28" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A28" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B28" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B28" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C28" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C28" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D28" s="12"/>
+      <c r="E28" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E28" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F28" s="9" t="str">
+        <f>IF($D28="","",A28&amp;RIGHT("00000"&amp;B28,5)&amp;C28&amp;"_"&amp;RIGHT("000"&amp;D28,3)&amp;E28)</f>
+        <v/>
+      </c>
+      <c r="G28" s="13" t="str">
+        <f>IF($D28="",G29&amp;"",F28&amp;IF(G29="","",IF(OR(G29=0,G29=""),"",","&amp;G29)))</f>
+        <v/>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A29" s="15" t="str">
-        <f>IF($E29="","",A28)</f>
-        <v/>
-      </c>
-      <c r="B29" s="15" t="str">
-        <f>IF($E29="","",B28)</f>
-        <v/>
-      </c>
-      <c r="C29" s="15" t="str">
-        <f>IF($E29="","",C28)</f>
-        <v/>
-      </c>
-      <c r="D29" s="15" t="str">
-        <f>IF($E29="","",D28)</f>
-        <v/>
-      </c>
-      <c r="E29" s="16"/>
-      <c r="F29" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G29" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="A29" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A29" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B29" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B29" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C29" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C29" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D29" s="12"/>
+      <c r="E29" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E29" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F29" s="9" t="str">
+        <f>IF($D29="","",A29&amp;RIGHT("00000"&amp;B29,5)&amp;C29&amp;"_"&amp;RIGHT("000"&amp;D29,3)&amp;E29)</f>
+        <v/>
+      </c>
+      <c r="G29" s="13" t="str">
+        <f>IF($D29="",G30&amp;"",F29&amp;IF(G30="","",IF(OR(G30=0,G30=""),"",","&amp;G30)))</f>
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A30" s="15" t="str">
-        <f>IF($E30="","",A29)</f>
-        <v/>
-      </c>
-      <c r="B30" s="15" t="str">
-        <f>IF($E30="","",B29)</f>
-        <v/>
-      </c>
-      <c r="C30" s="15" t="str">
-        <f>IF($E30="","",C29)</f>
-        <v/>
-      </c>
-      <c r="D30" s="15" t="str">
-        <f>IF($E30="","",D29)</f>
-        <v/>
-      </c>
-      <c r="E30" s="16"/>
-      <c r="F30" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G30" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="A30" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A30" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B30" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B30" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C30" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C30" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D30" s="12"/>
+      <c r="E30" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E30" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F30" s="9" t="str">
+        <f>IF($D30="","",A30&amp;RIGHT("00000"&amp;B30,5)&amp;C30&amp;"_"&amp;RIGHT("000"&amp;D30,3)&amp;E30)</f>
+        <v/>
+      </c>
+      <c r="G30" s="13" t="str">
+        <f>IF($D30="",G31&amp;"",F30&amp;IF(G31="","",IF(OR(G31=0,G31=""),"",","&amp;G31)))</f>
+        <v/>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A31" s="15" t="str">
-        <f>IF($E31="","",A30)</f>
-        <v/>
-      </c>
-      <c r="B31" s="15" t="str">
-        <f>IF($E31="","",B30)</f>
-        <v/>
-      </c>
-      <c r="C31" s="15" t="str">
-        <f>IF($E31="","",C30)</f>
-        <v/>
-      </c>
-      <c r="D31" s="15" t="str">
-        <f>IF($E31="","",D30)</f>
-        <v/>
-      </c>
-      <c r="E31" s="16"/>
-      <c r="F31" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G31" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="A31" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A31" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B31" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B31" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C31" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C31" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D31" s="12"/>
+      <c r="E31" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E31" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F31" s="9" t="str">
+        <f>IF($D31="","",A31&amp;RIGHT("00000"&amp;B31,5)&amp;C31&amp;"_"&amp;RIGHT("000"&amp;D31,3)&amp;E31)</f>
+        <v/>
+      </c>
+      <c r="G31" s="13" t="str">
+        <f>IF($D31="",G32&amp;"",F31&amp;IF(G32="","",IF(OR(G32=0,G32=""),"",","&amp;G32)))</f>
+        <v/>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A32" s="15" t="str">
-        <f>IF($E32="","",A31)</f>
-        <v/>
-      </c>
-      <c r="B32" s="15" t="str">
-        <f>IF($E32="","",B31)</f>
-        <v/>
-      </c>
-      <c r="C32" s="15" t="str">
-        <f>IF($E32="","",C31)</f>
-        <v/>
-      </c>
-      <c r="D32" s="15" t="str">
-        <f>IF($E32="","",D31)</f>
-        <v/>
-      </c>
-      <c r="E32" s="16"/>
-      <c r="F32" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G32" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="A32" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A32" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B32" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B32" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C32" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C32" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D32" s="12"/>
+      <c r="E32" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E32" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F32" s="9" t="str">
+        <f>IF($D32="","",A32&amp;RIGHT("00000"&amp;B32,5)&amp;C32&amp;"_"&amp;RIGHT("000"&amp;D32,3)&amp;E32)</f>
+        <v/>
+      </c>
+      <c r="G32" s="13" t="str">
+        <f>IF($D32="",G33&amp;"",F32&amp;IF(G33="","",IF(OR(G33=0,G33=""),"",","&amp;G33)))</f>
+        <v/>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A33" s="15" t="str">
-        <f>IF($E33="","",A32)</f>
-        <v/>
-      </c>
-      <c r="B33" s="15" t="str">
-        <f>IF($E33="","",B32)</f>
-        <v/>
-      </c>
-      <c r="C33" s="15" t="str">
-        <f>IF($E33="","",C32)</f>
-        <v/>
-      </c>
-      <c r="D33" s="15" t="str">
-        <f>IF($E33="","",D32)</f>
-        <v/>
-      </c>
-      <c r="E33" s="16"/>
-      <c r="F33" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G33" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="A33" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A33" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B33" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B33" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C33" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C33" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D33" s="12"/>
+      <c r="E33" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E33" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F33" s="9" t="str">
+        <f>IF($D33="","",A33&amp;RIGHT("00000"&amp;B33,5)&amp;C33&amp;"_"&amp;RIGHT("000"&amp;D33,3)&amp;E33)</f>
+        <v/>
+      </c>
+      <c r="G33" s="13" t="str">
+        <f>IF($D33="",G34&amp;"",F33&amp;IF(G34="","",IF(OR(G34=0,G34=""),"",","&amp;G34)))</f>
+        <v/>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A34" s="15" t="str">
-        <f>IF($E34="","",A33)</f>
-        <v/>
-      </c>
-      <c r="B34" s="15" t="str">
-        <f>IF($E34="","",B33)</f>
-        <v/>
-      </c>
-      <c r="C34" s="15" t="str">
-        <f>IF($E34="","",C33)</f>
-        <v/>
-      </c>
-      <c r="D34" s="15" t="str">
-        <f>IF($E34="","",D33)</f>
-        <v/>
-      </c>
-      <c r="E34" s="16"/>
-      <c r="F34" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G34" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="A34" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A34" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B34" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B34" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C34" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C34" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D34" s="12"/>
+      <c r="E34" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E34" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F34" s="9" t="str">
+        <f>IF($D34="","",A34&amp;RIGHT("00000"&amp;B34,5)&amp;C34&amp;"_"&amp;RIGHT("000"&amp;D34,3)&amp;E34)</f>
+        <v/>
+      </c>
+      <c r="G34" s="13" t="str">
+        <f>IF($D34="",G35&amp;"",F34&amp;IF(G35="","",IF(OR(G35=0,G35=""),"",","&amp;G35)))</f>
+        <v/>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A35" s="15" t="str">
-        <f>IF($E35="","",A34)</f>
-        <v/>
-      </c>
-      <c r="B35" s="15" t="str">
-        <f>IF($E35="","",B34)</f>
-        <v/>
-      </c>
-      <c r="C35" s="15" t="str">
-        <f>IF($E35="","",C34)</f>
-        <v/>
-      </c>
-      <c r="D35" s="15" t="str">
-        <f>IF($E35="","",D34)</f>
-        <v/>
-      </c>
-      <c r="E35" s="16"/>
-      <c r="F35" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G35" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="A35" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A35" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B35" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B35" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C35" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C35" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D35" s="12"/>
+      <c r="E35" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E35" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F35" s="9" t="str">
+        <f>IF($D35="","",A35&amp;RIGHT("00000"&amp;B35,5)&amp;C35&amp;"_"&amp;RIGHT("000"&amp;D35,3)&amp;E35)</f>
+        <v/>
+      </c>
+      <c r="G35" s="13" t="str">
+        <f>IF($D35="",G36&amp;"",F35&amp;IF(G36="","",IF(OR(G36=0,G36=""),"",","&amp;G36)))</f>
+        <v/>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A36" s="15" t="str">
-        <f>IF($E36="","",A35)</f>
-        <v/>
-      </c>
-      <c r="B36" s="15" t="str">
-        <f>IF($E36="","",B35)</f>
-        <v/>
-      </c>
-      <c r="C36" s="15" t="str">
-        <f>IF($E36="","",C35)</f>
-        <v/>
-      </c>
-      <c r="D36" s="15" t="str">
-        <f>IF($E36="","",D35)</f>
-        <v/>
-      </c>
-      <c r="E36" s="16"/>
-      <c r="F36" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G36" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="A36" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A36" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B36" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B36" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C36" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C36" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D36" s="12"/>
+      <c r="E36" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E36" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F36" s="9" t="str">
+        <f>IF($D36="","",A36&amp;RIGHT("00000"&amp;B36,5)&amp;C36&amp;"_"&amp;RIGHT("000"&amp;D36,3)&amp;E36)</f>
+        <v/>
+      </c>
+      <c r="G36" s="13" t="str">
+        <f>IF($D36="",G37&amp;"",F36&amp;IF(G37="","",IF(OR(G37=0,G37=""),"",","&amp;G37)))</f>
+        <v/>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A37" s="15" t="str">
-        <f>IF($E37="","",A36)</f>
-        <v/>
-      </c>
-      <c r="B37" s="15" t="str">
-        <f>IF($E37="","",B36)</f>
-        <v/>
-      </c>
-      <c r="C37" s="15" t="str">
-        <f>IF($E37="","",C36)</f>
-        <v/>
-      </c>
-      <c r="D37" s="15" t="str">
-        <f>IF($E37="","",D36)</f>
-        <v/>
-      </c>
-      <c r="E37" s="16"/>
-      <c r="F37" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G37" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="A37" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A37" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B37" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B37" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C37" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C37" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D37" s="12"/>
+      <c r="E37" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E37" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F37" s="9" t="str">
+        <f>IF($D37="","",A37&amp;RIGHT("00000"&amp;B37,5)&amp;C37&amp;"_"&amp;RIGHT("000"&amp;D37,3)&amp;E37)</f>
+        <v/>
+      </c>
+      <c r="G37" s="13" t="str">
+        <f>IF($D37="",G38&amp;"",F37&amp;IF(G38="","",IF(OR(G38=0,G38=""),"",","&amp;G38)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A38" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A38" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B38" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B38" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C38" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C38" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D38" s="12"/>
+      <c r="E38" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E38" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F38" s="9" t="str">
+        <f>IF($D38="","",A38&amp;RIGHT("00000"&amp;B38,5)&amp;C38&amp;"_"&amp;RIGHT("000"&amp;D38,3)&amp;E38)</f>
+        <v/>
+      </c>
+      <c r="G38" s="13" t="str">
+        <f>IF($D38="",G39&amp;"",F38&amp;IF(G39="","",IF(OR(G39=0,G39=""),"",","&amp;G39)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A39" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A39" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B39" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B39" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C39" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C39" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D39" s="12"/>
+      <c r="E39" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E39" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F39" s="9" t="str">
+        <f>IF($D39="","",A39&amp;RIGHT("00000"&amp;B39,5)&amp;C39&amp;"_"&amp;RIGHT("000"&amp;D39,3)&amp;E39)</f>
+        <v/>
+      </c>
+      <c r="G39" s="13" t="str">
+        <f>IF($D39="",G40&amp;"",F39&amp;IF(G40="","",IF(OR(G40=0,G40=""),"",","&amp;G40)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A40" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A40" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B40" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B40" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C40" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C40" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D40" s="12"/>
+      <c r="E40" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E40" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F40" s="9" t="str">
+        <f>IF($D40="","",A40&amp;RIGHT("00000"&amp;B40,5)&amp;C40&amp;"_"&amp;RIGHT("000"&amp;D40,3)&amp;E40)</f>
+        <v/>
+      </c>
+      <c r="G40" s="13" t="str">
+        <f>IF($D40="",G41&amp;"",F40&amp;IF(G41="","",IF(OR(G41=0,G41=""),"",","&amp;G41)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A41" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A41" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B41" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B41" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C41" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C41" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D41" s="12"/>
+      <c r="E41" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E41" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F41" s="9" t="str">
+        <f>IF($D41="","",A41&amp;RIGHT("00000"&amp;B41,5)&amp;C41&amp;"_"&amp;RIGHT("000"&amp;D41,3)&amp;E41)</f>
+        <v/>
+      </c>
+      <c r="G41" s="13" t="str">
+        <f>IF($D41="",G42&amp;"",F41&amp;IF(G42="","",IF(OR(G42=0,G42=""),"",","&amp;G42)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A42" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A42" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B42" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B42" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C42" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C42" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D42" s="15"/>
+      <c r="E42" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E42" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F42" s="9" t="str">
+        <f>IF($D42="","",A42&amp;RIGHT("00000"&amp;B42,5)&amp;C42&amp;"_"&amp;RIGHT("000"&amp;D42,3)&amp;E42)</f>
+        <v/>
+      </c>
+      <c r="G42" s="13" t="str">
+        <f>IF($D42="",G43&amp;"",F42&amp;IF(G43="","",IF(OR(G43=0,G43=""),"",","&amp;G43)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A43" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A43" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B43" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B43" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C43" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C43" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D43" s="15"/>
+      <c r="E43" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E43" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F43" s="9" t="str">
+        <f>IF($D43="","",A43&amp;RIGHT("00000"&amp;B43,5)&amp;C43&amp;"_"&amp;RIGHT("000"&amp;D43,3)&amp;E43)</f>
+        <v/>
+      </c>
+      <c r="G43" s="13" t="str">
+        <f>IF($D43="",G44&amp;"",F43&amp;IF(G44="","",IF(OR(G44=0,G44=""),"",","&amp;G44)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A44" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A44" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B44" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B44" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C44" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C44" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D44" s="15"/>
+      <c r="E44" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E44" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F44" s="9" t="str">
+        <f>IF($D44="","",A44&amp;RIGHT("00000"&amp;B44,5)&amp;C44&amp;"_"&amp;RIGHT("000"&amp;D44,3)&amp;E44)</f>
+        <v/>
+      </c>
+      <c r="G44" s="13" t="str">
+        <f>IF($D44="",G45&amp;"",F44&amp;IF(G45="","",IF(OR(G45=0,G45=""),"",","&amp;G45)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A45" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A45" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B45" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B45" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C45" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C45" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D45" s="15"/>
+      <c r="E45" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E45" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F45" s="9" t="str">
+        <f>IF($D45="","",A45&amp;RIGHT("00000"&amp;B45,5)&amp;C45&amp;"_"&amp;RIGHT("000"&amp;D45,3)&amp;E45)</f>
+        <v/>
+      </c>
+      <c r="G45" s="13" t="str">
+        <f>IF($D45="",G46&amp;"",F45&amp;IF(G46="","",IF(OR(G46=0,G46=""),"",","&amp;G46)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A46" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A46" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B46" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B46" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C46" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C46" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D46" s="15"/>
+      <c r="E46" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E46" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F46" s="9" t="str">
+        <f>IF($D46="","",A46&amp;RIGHT("00000"&amp;B46,5)&amp;C46&amp;"_"&amp;RIGHT("000"&amp;D46,3)&amp;E46)</f>
+        <v/>
+      </c>
+      <c r="G46" s="13" t="str">
+        <f>IF($D46="",G47&amp;"",F46&amp;IF(G47="","",IF(OR(G47=0,G47=""),"",","&amp;G47)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A47" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A47" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B47" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B47" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C47" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C47" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D47" s="15"/>
+      <c r="E47" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E47" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F47" s="9" t="str">
+        <f>IF($D47="","",A47&amp;RIGHT("00000"&amp;B47,5)&amp;C47&amp;"_"&amp;RIGHT("000"&amp;D47,3)&amp;E47)</f>
+        <v/>
+      </c>
+      <c r="G47" s="13" t="str">
+        <f>IF($D47="",G48&amp;"",F47&amp;IF(G48="","",IF(OR(G48=0,G48=""),"",","&amp;G48)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A48" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A48" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B48" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B48" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C48" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C48" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D48" s="15"/>
+      <c r="E48" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E48" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F48" s="9" t="str">
+        <f>IF($D48="","",A48&amp;RIGHT("00000"&amp;B48,5)&amp;C48&amp;"_"&amp;RIGHT("000"&amp;D48,3)&amp;E48)</f>
+        <v/>
+      </c>
+      <c r="G48" s="13" t="str">
+        <f>IF($D48="",G49&amp;"",F48&amp;IF(G49="","",IF(OR(G49=0,G49=""),"",","&amp;G49)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A49" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A49" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B49" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B49" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C49" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C49" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D49" s="15"/>
+      <c r="E49" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E49" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F49" s="9" t="str">
+        <f>IF($D49="","",A49&amp;RIGHT("00000"&amp;B49,5)&amp;C49&amp;"_"&amp;RIGHT("000"&amp;D49,3)&amp;E49)</f>
+        <v/>
+      </c>
+      <c r="G49" s="13" t="str">
+        <f>IF($D49="",G50&amp;"",F49&amp;IF(G50="","",IF(OR(G50=0,G50=""),"",","&amp;G50)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A50" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A50" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B50" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B50" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C50" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C50" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D50" s="15"/>
+      <c r="E50" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E50" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F50" s="9" t="str">
+        <f>IF($D50="","",A50&amp;RIGHT("00000"&amp;B50,5)&amp;C50&amp;"_"&amp;RIGHT("000"&amp;D50,3)&amp;E50)</f>
+        <v/>
+      </c>
+      <c r="G50" s="13" t="str">
+        <f>IF($D50="",G51&amp;"",F50&amp;IF(G51="","",IF(OR(G51=0,G51=""),"",","&amp;G51)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A51" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A51" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B51" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B51" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C51" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C51" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D51" s="15"/>
+      <c r="E51" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E51" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F51" s="9" t="str">
+        <f>IF($D51="","",A51&amp;RIGHT("00000"&amp;B51,5)&amp;C51&amp;"_"&amp;RIGHT("000"&amp;D51,3)&amp;E51)</f>
+        <v/>
+      </c>
+      <c r="G51" s="13" t="str">
+        <f>IF($D51="",G52&amp;"",F51&amp;IF(G52="","",IF(OR(G52=0,G52=""),"",","&amp;G52)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A52" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A52" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B52" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B52" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C52" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C52" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D52" s="15"/>
+      <c r="E52" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E52" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F52" s="9" t="str">
+        <f>IF($D52="","",A52&amp;RIGHT("00000"&amp;B52,5)&amp;C52&amp;"_"&amp;RIGHT("000"&amp;D52,3)&amp;E52)</f>
+        <v/>
+      </c>
+      <c r="G52" s="13" t="str">
+        <f>IF($D52="",G53&amp;"",F52&amp;IF(G53="","",IF(OR(G53=0,G53=""),"",","&amp;G53)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A53" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A53" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B53" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B53" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C53" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C53" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D53" s="15"/>
+      <c r="E53" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E53" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F53" s="9" t="str">
+        <f>IF($D53="","",A53&amp;RIGHT("00000"&amp;B53,5)&amp;C53&amp;"_"&amp;RIGHT("000"&amp;D53,3)&amp;E53)</f>
+        <v/>
+      </c>
+      <c r="G53" s="13" t="str">
+        <f>IF($D53="",G54&amp;"",F53&amp;IF(G54="","",IF(OR(G54=0,G54=""),"",","&amp;G54)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A54" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A54" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B54" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B54" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C54" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C54" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D54" s="15"/>
+      <c r="E54" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E54" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F54" s="9" t="str">
+        <f>IF($D54="","",A54&amp;RIGHT("00000"&amp;B54,5)&amp;C54&amp;"_"&amp;RIGHT("000"&amp;D54,3)&amp;E54)</f>
+        <v/>
+      </c>
+      <c r="G54" s="13" t="str">
+        <f>IF($D54="",G55&amp;"",F54&amp;IF(G55="","",IF(OR(G55=0,G55=""),"",","&amp;G55)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A55" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A55" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B55" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B55" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C55" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C55" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D55" s="15"/>
+      <c r="E55" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E55" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F55" s="9" t="str">
+        <f>IF($D55="","",A55&amp;RIGHT("00000"&amp;B55,5)&amp;C55&amp;"_"&amp;RIGHT("000"&amp;D55,3)&amp;E55)</f>
+        <v/>
+      </c>
+      <c r="G55" s="13" t="str">
+        <f>IF($D55="",G56&amp;"",F55&amp;IF(G56="","",IF(OR(G56=0,G56=""),"",","&amp;G56)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A56" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A56" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B56" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B56" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C56" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C56" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D56" s="15"/>
+      <c r="E56" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E56" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F56" s="9" t="str">
+        <f>IF($D56="","",A56&amp;RIGHT("00000"&amp;B56,5)&amp;C56&amp;"_"&amp;RIGHT("000"&amp;D56,3)&amp;E56)</f>
+        <v/>
+      </c>
+      <c r="G56" s="13" t="str">
+        <f>IF($D56="",G57&amp;"",F56&amp;IF(G57="","",IF(OR(G57=0,G57=""),"",","&amp;G57)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A57" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A57" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B57" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B57" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C57" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C57" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D57" s="15"/>
+      <c r="E57" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E57" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F57" s="9" t="str">
+        <f>IF($D57="","",A57&amp;RIGHT("00000"&amp;B57,5)&amp;C57&amp;"_"&amp;RIGHT("000"&amp;D57,3)&amp;E57)</f>
+        <v/>
+      </c>
+      <c r="G57" s="13" t="str">
+        <f>IF($D57="",G58&amp;"",F57&amp;IF(G58="","",IF(OR(G58=0,G58=""),"",","&amp;G58)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A58" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A58" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B58" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B58" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C58" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C58" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D58" s="15"/>
+      <c r="E58" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E58" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F58" s="9" t="str">
+        <f>IF($D58="","",A58&amp;RIGHT("00000"&amp;B58,5)&amp;C58&amp;"_"&amp;RIGHT("000"&amp;D58,3)&amp;E58)</f>
+        <v/>
+      </c>
+      <c r="G58" s="13" t="str">
+        <f>IF($D58="",G59&amp;"",F58&amp;IF(G59="","",IF(OR(G59=0,G59=""),"",","&amp;G59)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A59" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A59" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B59" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B59" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C59" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C59" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D59" s="15"/>
+      <c r="E59" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E59" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F59" s="9" t="str">
+        <f>IF($D59="","",A59&amp;RIGHT("00000"&amp;B59,5)&amp;C59&amp;"_"&amp;RIGHT("000"&amp;D59,3)&amp;E59)</f>
+        <v/>
+      </c>
+      <c r="G59" s="13" t="str">
+        <f>IF($D59="",G60&amp;"",F59&amp;IF(G60="","",IF(OR(G60=0,G60=""),"",","&amp;G60)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A60" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A60" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B60" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B60" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C60" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C60" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D60" s="15"/>
+      <c r="E60" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E60" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F60" s="9" t="str">
+        <f>IF($D60="","",A60&amp;RIGHT("00000"&amp;B60,5)&amp;C60&amp;"_"&amp;RIGHT("000"&amp;D60,3)&amp;E60)</f>
+        <v/>
+      </c>
+      <c r="G60" s="13" t="str">
+        <f>IF($D60="",G61&amp;"",F60&amp;IF(G61="","",IF(OR(G61=0,G61=""),"",","&amp;G61)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A61" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A61" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B61" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B61" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C61" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C61" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D61" s="15"/>
+      <c r="E61" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E61" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F61" s="9" t="str">
+        <f>IF($D61="","",A61&amp;RIGHT("00000"&amp;B61,5)&amp;C61&amp;"_"&amp;RIGHT("000"&amp;D61,3)&amp;E61)</f>
+        <v/>
+      </c>
+      <c r="G61" s="13" t="str">
+        <f>IF($D61="",G62&amp;"",F61&amp;IF(G62="","",IF(OR(G62=0,G62=""),"",","&amp;G62)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A62" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="A62" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>B</v>
+      </c>
+      <c r="B62" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="B62" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>11001</v>
+      </c>
+      <c r="C62" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="C62" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v/>
+      </c>
+      <c r="D62" s="15"/>
+      <c r="E62" s="14" t="str" cm="1">
+        <f t="array" aca="1" ref="E62" ca="1">OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),-1,0)&amp;""</f>
+        <v>E</v>
+      </c>
+      <c r="F62" s="9" t="str">
+        <f>IF($D62="","",A62&amp;RIGHT("00000"&amp;B62,5)&amp;C62&amp;"_"&amp;RIGHT("000"&amp;D62,3)&amp;E62)</f>
+        <v/>
+      </c>
+      <c r="G62" s="13" t="str">
+        <f>IF($D62="",G63&amp;"",F62&amp;IF(G63="","",IF(OR(G63=0,G63=""),"",","&amp;G63)))</f>
+        <v/>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="I10:M11"/>
+    <mergeCell ref="I7:M7"/>
+    <mergeCell ref="I12:M12"/>
+    <mergeCell ref="I5:M5"/>
+    <mergeCell ref="I6:M6"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B2:G4"/>
+    <mergeCell ref="I2:M3"/>
+    <mergeCell ref="I4:M4"/>
+    <mergeCell ref="I8:M9"/>
+    <mergeCell ref="I1:M1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A14:E62">
+    <cfRule type="expression" dxfId="5" priority="13" stopIfTrue="1">
+      <formula>A14&amp;""&lt;&gt;A13&amp;""</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="14">
+      <formula>$D14&amp;""=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A39:C39 E39">
+    <cfRule type="expression" dxfId="3" priority="19" stopIfTrue="1">
+      <formula>A39&amp;""&lt;&gt;A18&amp;""</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="20">
+      <formula>$D39&amp;""=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29:C29 E29">
+    <cfRule type="expression" dxfId="1" priority="21" stopIfTrue="1">
+      <formula>A29&amp;""&lt;&gt;A18&amp;""</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="22">
+      <formula>$D29&amp;""=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="P4" r:id="rId1" xr:uid="{1AA27F17-099A-E44B-9216-3DDD57A284AB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2017,7 +3684,7 @@
   <dimension ref="A2:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -2026,14 +3693,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A2" s="17" t="s">
-        <v>232</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>233</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>231</v>
+      <c r="A2" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1">
@@ -2166,6 +3833,12 @@
       </c>
       <c r="C14" s="2" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1">
+      <c r="C16" s="7" t="str">
+        <f>C18&amp;H23&amp;C19</f>
+        <v>https://api.census.gov/data/2018/acs/acs5?get=B19013_001E,B19013A_001E,B19013B_001E,B19013C_001E,B19013D_001E,B19013E_001E,B19013F_001E,B19013G_001E,B19013H_001E,B19013I_001E&amp;for=block%20group:*&amp;in=state:48&amp;in=county:029&amp;in=tract:*</v>
       </c>
     </row>
     <row r="17" spans="3:3" ht="15.75" customHeight="1">
@@ -2204,7 +3877,7 @@
   <dimension ref="A2:X182"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>